<commit_message>
Lab testing report finalized
</commit_message>
<xml_diff>
--- a/TestingFile.xlsx
+++ b/TestingFile.xlsx
@@ -108,10 +108,10 @@
     <t>Muhamamd Ali</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
     <t>Fabric</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +544,7 @@
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>12</v>
+        <v>200</v>
       </c>
       <c r="B2" s="2">
         <v>44515</v>
@@ -568,10 +568,10 @@
         <v>1590</v>
       </c>
       <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
         <v>25</v>
-      </c>
-      <c r="J2" t="s">
-        <v>26</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>4</v>
@@ -613,6 +613,12 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K6" t="s">
         <v>12</v>
+      </c>
+      <c r="L6">
+        <v>200</v>
+      </c>
+      <c r="M6">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>